<commit_message>
More on linear regression
</commit_message>
<xml_diff>
--- a/Data/US_em.xlsx
+++ b/Data/US_em.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IsaacEvans\Documents\Uni\AI\EV_affect_on_emissions\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Liu2286\Documents\GitHub\EV_affect_on_emissions\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2C89FD44-E1CE-4B1A-8D8D-147AA11C886A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91EADEFE-E450-4413-866C-028697EA3631}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="US_em" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="21">
   <si>
     <t>Gas/Vehicle</t>
   </si>
@@ -84,57 +84,30 @@
   <si>
     <t>Biodiesel CO2 g</t>
   </si>
-  <si>
-    <t>Notes: Passenger cars and light-duty trucks include vehicles typically used for personal travel and less than 8,500 lbs; medium- and heavy-duty trucks include vehicles larger than 8,500 lbs. HFC emissions primarily reflect HFC-134a. Totals may not sum due to independent rounding.</t>
-  </si>
-  <si>
-    <t>+ Does not exceed 0.05 MMT CO2 Eq.</t>
-  </si>
-  <si>
-    <t>a Consists of emissions from jet fuel consumed by domestic operations of commercial aircraft (no bunkers).</t>
-  </si>
-  <si>
-    <t>b Consists of emissions from jet fuel and aviation gasoline consumption by general aviation and military aircraft.</t>
-  </si>
-  <si>
-    <t>c Fluctuations in emission estimates are associated with fluctuations in reported fuel consumption and may reflect issues with data sources.</t>
-  </si>
-  <si>
-    <t>d Other emissions from electric power are a result of waste incineration (as the majority of municipal solid waste is combusted in “trash-to-steam” electric power plants), electrical transmission and distribution, and a portion of Other Process Uses of Carbonates (from pollution control equipment installed in electric power plants).</t>
-  </si>
-  <si>
-    <t>e CO2 estimates reflect natural gas used to power pipelines, but not electricity. While the operation of pipelines produces CH4 and N2O, these emissions are not directly attributed to pipelines in the Inventory.</t>
-  </si>
-  <si>
-    <t>f Emissions from International Bunker Fuels include emissions from both civilian and military activities; these emissions are not included in the transportation totals.</t>
-  </si>
-  <si>
-    <t>g Ethanol and biodiesel CO2 estimates are presented for informational purposes only. See Section 3.11 and the estimates in Land Use, Land-Use Change, and Forestry (see Chapter 6), in line with IPCC methodological guidance and UNFCCC reporting obligations, for more information on ethanol and biodiesel.</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="18"/>
       <color theme="3"/>
-      <name val="Calibri Light"/>
+      <name val="等线 Light"/>
       <family val="2"/>
       <scheme val="major"/>
     </font>
@@ -142,7 +115,7 @@
       <b/>
       <sz val="15"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -150,7 +123,7 @@
       <b/>
       <sz val="13"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -158,35 +131,35 @@
       <b/>
       <sz val="11"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C5700"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -194,7 +167,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -202,14 +175,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -217,14 +190,14 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -232,7 +205,7 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -240,15 +213,22 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -950,16 +930,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE60"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AE50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="AG55" sqref="AG55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="54.25" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1054,7 +1037,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1149,7 +1132,7 @@
         <v>762.3</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1244,7 +1227,7 @@
         <v>748.3</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1339,7 +1322,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1434,7 +1417,7 @@
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1529,7 +1512,7 @@
         <v>9.3000000000000007</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1624,7 +1607,7 @@
         <v>323.10000000000002</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -1719,7 +1702,7 @@
         <v>304.3</v>
       </c>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -1814,7 +1797,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -1909,7 +1892,7 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -2004,7 +1987,7 @@
         <v>16.899999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -2099,7 +2082,7 @@
         <v>444.4</v>
       </c>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -2194,7 +2177,7 @@
         <v>435.2</v>
       </c>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>3</v>
       </c>
@@ -2289,7 +2272,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>4</v>
       </c>
@@ -2384,7 +2367,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>5</v>
       </c>
@@ -2479,7 +2462,7 @@
         <v>6.1</v>
       </c>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>8</v>
       </c>
@@ -2574,7 +2557,7 @@
         <v>22.2</v>
       </c>
     </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>2</v>
       </c>
@@ -2669,7 +2652,7 @@
         <v>21.4</v>
       </c>
     </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>3</v>
       </c>
@@ -2764,7 +2747,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>4</v>
       </c>
@@ -2859,7 +2842,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>5</v>
       </c>
@@ -2954,7 +2937,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>10</v>
       </c>
@@ -3049,7 +3032,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>2</v>
       </c>
@@ -3144,7 +3127,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>3</v>
       </c>
@@ -3239,7 +3222,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>4</v>
       </c>
@@ -3334,7 +3317,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>11</v>
       </c>
@@ -3429,7 +3412,7 @@
         <v>135.4</v>
       </c>
     </row>
-    <row r="27" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>2</v>
       </c>
@@ -3524,7 +3507,7 @@
         <v>134.19999999999999</v>
       </c>
     </row>
-    <row r="28" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>3</v>
       </c>
@@ -3619,7 +3602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>4</v>
       </c>
@@ -3714,7 +3697,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="30" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>12</v>
       </c>
@@ -3809,7 +3792,7 @@
         <v>45.7</v>
       </c>
     </row>
-    <row r="31" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>2</v>
       </c>
@@ -3904,7 +3887,7 @@
         <v>45.2</v>
       </c>
     </row>
-    <row r="32" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>3</v>
       </c>
@@ -3999,7 +3982,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>4</v>
       </c>
@@ -4094,7 +4077,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="34" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>13</v>
       </c>
@@ -4189,7 +4172,7 @@
         <v>40.4</v>
       </c>
     </row>
-    <row r="35" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>2</v>
       </c>
@@ -4284,7 +4267,7 @@
         <v>35.9</v>
       </c>
     </row>
-    <row r="36" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>3</v>
       </c>
@@ -4379,7 +4362,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="37" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>4</v>
       </c>
@@ -4474,7 +4457,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="38" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>5</v>
       </c>
@@ -4569,7 +4552,7 @@
         <v>3.9</v>
       </c>
     </row>
-    <row r="39" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>14</v>
       </c>
@@ -4664,7 +4647,7 @@
         <v>40.799999999999997</v>
       </c>
     </row>
-    <row r="40" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>2</v>
       </c>
@@ -4759,7 +4742,7 @@
         <v>40.200000000000003</v>
       </c>
     </row>
-    <row r="41" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>3</v>
       </c>
@@ -4854,7 +4837,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="42" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>4</v>
       </c>
@@ -4949,7 +4932,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="43" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>5</v>
       </c>
@@ -5044,7 +5027,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="44" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>15</v>
       </c>
@@ -5139,7 +5122,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="45" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>16</v>
       </c>
@@ -5234,7 +5217,7 @@
         <v>53.7</v>
       </c>
     </row>
-    <row r="46" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>2</v>
       </c>
@@ -5329,7 +5312,7 @@
         <v>53.7</v>
       </c>
     </row>
-    <row r="47" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>17</v>
       </c>
@@ -5424,7 +5407,7 @@
         <v>1871.7</v>
       </c>
     </row>
-    <row r="48" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>18</v>
       </c>
@@ -5519,7 +5502,7 @@
         <v>26.4</v>
       </c>
     </row>
-    <row r="49" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>19</v>
       </c>
@@ -5614,7 +5597,7 @@
         <v>78.7</v>
       </c>
     </row>
-    <row r="50" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>20</v>
       </c>
@@ -5709,52 +5692,9 @@
         <v>17.100000000000001</v>
       </c>
     </row>
-    <row r="52" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="53" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="54" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="55" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="56" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="57" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A57" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="58" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A58" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="59" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="60" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A60" t="s">
-        <v>29</v>
-      </c>
-    </row>
   </sheetData>
+  <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
working for other emissions datasets
</commit_message>
<xml_diff>
--- a/Data/US_em.xlsx
+++ b/Data/US_em.xlsx
@@ -1,29 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Liu2286\Documents\GitHub\EV_affect_on_emissions\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IsaacEvans\Documents\Uni\AI\EV_affect_on_emissions\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91EADEFE-E450-4413-866C-028697EA3631}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DD1BAD0-2F1F-4A73-A9B4-C0E02F3A9003}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="US_em" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="21">
-  <si>
-    <t>Gas/Vehicle</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="21">
   <si>
     <t>Passenger Cars</t>
   </si>
@@ -84,30 +92,33 @@
   <si>
     <t>Biodiesel CO2 g</t>
   </si>
+  <si>
+    <t>Year</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="18"/>
       <color theme="3"/>
-      <name val="等线 Light"/>
+      <name val="Calibri Light"/>
       <family val="2"/>
       <scheme val="major"/>
     </font>
@@ -115,7 +126,7 @@
       <b/>
       <sz val="15"/>
       <color theme="3"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -123,7 +134,7 @@
       <b/>
       <sz val="13"/>
       <color theme="3"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -131,35 +142,35 @@
       <b/>
       <sz val="11"/>
       <color theme="3"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C5700"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -167,7 +178,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -175,14 +186,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -190,14 +201,14 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -205,7 +216,7 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -213,20 +224,20 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -933,18 +944,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="AG55" sqref="AG55"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="54.25" customWidth="1"/>
+    <col min="1" max="1" width="54.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:31">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="B1">
         <v>1990</v>
@@ -1037,9 +1046,9 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:31">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
         <v>639.6</v>
@@ -1132,9 +1141,9 @@
         <v>762.3</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:31">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>612.20000000000005</v>
@@ -1227,9 +1236,9 @@
         <v>748.3</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:31">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>3.2</v>
@@ -1322,9 +1331,9 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:31">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>24.1</v>
@@ -1417,9 +1426,9 @@
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:31">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -1512,9 +1521,9 @@
         <v>9.3000000000000007</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:31">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
         <v>326.7</v>
@@ -1607,9 +1616,9 @@
         <v>323.10000000000002</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:31">
       <c r="A8" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B8">
         <v>312.2</v>
@@ -1702,9 +1711,9 @@
         <v>304.3</v>
       </c>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:31">
       <c r="A9" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B9">
         <v>1.7</v>
@@ -1797,9 +1806,9 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:31">
       <c r="A10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B10">
         <v>12.8</v>
@@ -1892,9 +1901,9 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:31">
       <c r="A11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -1987,9 +1996,9 @@
         <v>16.899999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:31">
       <c r="A12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B12">
         <v>230.3</v>
@@ -2082,9 +2091,9 @@
         <v>444.4</v>
       </c>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:31">
       <c r="A13" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B13">
         <v>229.3</v>
@@ -2177,9 +2186,9 @@
         <v>435.2</v>
       </c>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:31">
       <c r="A14" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B14">
         <v>0.3</v>
@@ -2272,9 +2281,9 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:31">
       <c r="A15" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B15">
         <v>0.7</v>
@@ -2367,9 +2376,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:31">
       <c r="A16" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -2462,9 +2471,9 @@
         <v>6.1</v>
       </c>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:31">
       <c r="A17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B17">
         <v>8.5</v>
@@ -2557,9 +2566,9 @@
         <v>22.2</v>
       </c>
     </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:31">
       <c r="A18" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B18">
         <v>8.4</v>
@@ -2652,39 +2661,39 @@
         <v>21.4</v>
       </c>
     </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:31">
       <c r="A19" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B19" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C19" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D19" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E19" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F19" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G19" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H19" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I19" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J19" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="K19" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="L19">
         <v>0.1</v>
@@ -2747,125 +2756,125 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:31">
       <c r="A20" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" t="s">
+        <v>8</v>
+      </c>
+      <c r="F20" t="s">
+        <v>8</v>
+      </c>
+      <c r="G20" t="s">
+        <v>8</v>
+      </c>
+      <c r="H20" t="s">
+        <v>8</v>
+      </c>
+      <c r="I20" t="s">
+        <v>8</v>
+      </c>
+      <c r="J20" t="s">
+        <v>8</v>
+      </c>
+      <c r="K20" t="s">
+        <v>8</v>
+      </c>
+      <c r="L20" t="s">
+        <v>8</v>
+      </c>
+      <c r="M20" t="s">
+        <v>8</v>
+      </c>
+      <c r="N20" t="s">
+        <v>8</v>
+      </c>
+      <c r="O20" t="s">
+        <v>8</v>
+      </c>
+      <c r="P20" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>8</v>
+      </c>
+      <c r="R20" t="s">
+        <v>8</v>
+      </c>
+      <c r="S20" t="s">
+        <v>8</v>
+      </c>
+      <c r="T20">
+        <v>0.1</v>
+      </c>
+      <c r="U20">
+        <v>0.1</v>
+      </c>
+      <c r="V20">
+        <v>0.1</v>
+      </c>
+      <c r="W20">
+        <v>0.1</v>
+      </c>
+      <c r="X20">
+        <v>0.1</v>
+      </c>
+      <c r="Y20">
+        <v>0.1</v>
+      </c>
+      <c r="Z20">
+        <v>0.1</v>
+      </c>
+      <c r="AA20">
+        <v>0.1</v>
+      </c>
+      <c r="AB20">
+        <v>0.1</v>
+      </c>
+      <c r="AC20">
+        <v>0.1</v>
+      </c>
+      <c r="AD20">
+        <v>0.1</v>
+      </c>
+      <c r="AE20">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:31">
+      <c r="A21" t="s">
         <v>4</v>
       </c>
-      <c r="B20" t="s">
-        <v>9</v>
-      </c>
-      <c r="C20" t="s">
-        <v>9</v>
-      </c>
-      <c r="D20" t="s">
-        <v>9</v>
-      </c>
-      <c r="E20" t="s">
-        <v>9</v>
-      </c>
-      <c r="F20" t="s">
-        <v>9</v>
-      </c>
-      <c r="G20" t="s">
-        <v>9</v>
-      </c>
-      <c r="H20" t="s">
-        <v>9</v>
-      </c>
-      <c r="I20" t="s">
-        <v>9</v>
-      </c>
-      <c r="J20" t="s">
-        <v>9</v>
-      </c>
-      <c r="K20" t="s">
-        <v>9</v>
-      </c>
-      <c r="L20" t="s">
-        <v>9</v>
-      </c>
-      <c r="M20" t="s">
-        <v>9</v>
-      </c>
-      <c r="N20" t="s">
-        <v>9</v>
-      </c>
-      <c r="O20" t="s">
-        <v>9</v>
-      </c>
-      <c r="P20" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q20" t="s">
-        <v>9</v>
-      </c>
-      <c r="R20" t="s">
-        <v>9</v>
-      </c>
-      <c r="S20" t="s">
-        <v>9</v>
-      </c>
-      <c r="T20">
-        <v>0.1</v>
-      </c>
-      <c r="U20">
-        <v>0.1</v>
-      </c>
-      <c r="V20">
-        <v>0.1</v>
-      </c>
-      <c r="W20">
-        <v>0.1</v>
-      </c>
-      <c r="X20">
-        <v>0.1</v>
-      </c>
-      <c r="Y20">
-        <v>0.1</v>
-      </c>
-      <c r="Z20">
-        <v>0.1</v>
-      </c>
-      <c r="AA20">
-        <v>0.1</v>
-      </c>
-      <c r="AB20">
-        <v>0.1</v>
-      </c>
-      <c r="AC20">
-        <v>0.1</v>
-      </c>
-      <c r="AD20">
-        <v>0.1</v>
-      </c>
-      <c r="AE20">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>5</v>
-      </c>
-      <c r="B21">
-        <v>0</v>
-      </c>
-      <c r="C21">
-        <v>0</v>
-      </c>
-      <c r="D21">
-        <v>0</v>
-      </c>
-      <c r="E21">
-        <v>0</v>
+      <c r="B21" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21" t="s">
+        <v>8</v>
       </c>
       <c r="F21" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G21" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H21" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I21">
         <v>0.1</v>
@@ -2937,9 +2946,9 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:31">
       <c r="A22" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B22">
         <v>1.7</v>
@@ -3032,9 +3041,9 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:31">
       <c r="A23" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B23">
         <v>1.7</v>
@@ -3127,199 +3136,199 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:31">
       <c r="A24" t="s">
+        <v>2</v>
+      </c>
+      <c r="B24" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" t="s">
+        <v>8</v>
+      </c>
+      <c r="D24" t="s">
+        <v>8</v>
+      </c>
+      <c r="E24" t="s">
+        <v>8</v>
+      </c>
+      <c r="F24" t="s">
+        <v>8</v>
+      </c>
+      <c r="G24" t="s">
+        <v>8</v>
+      </c>
+      <c r="H24" t="s">
+        <v>8</v>
+      </c>
+      <c r="I24" t="s">
+        <v>8</v>
+      </c>
+      <c r="J24" t="s">
+        <v>8</v>
+      </c>
+      <c r="K24" t="s">
+        <v>8</v>
+      </c>
+      <c r="L24" t="s">
+        <v>8</v>
+      </c>
+      <c r="M24" t="s">
+        <v>8</v>
+      </c>
+      <c r="N24" t="s">
+        <v>8</v>
+      </c>
+      <c r="O24" t="s">
+        <v>8</v>
+      </c>
+      <c r="P24" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>8</v>
+      </c>
+      <c r="R24" t="s">
+        <v>8</v>
+      </c>
+      <c r="S24" t="s">
+        <v>8</v>
+      </c>
+      <c r="T24" t="s">
+        <v>8</v>
+      </c>
+      <c r="U24" t="s">
+        <v>8</v>
+      </c>
+      <c r="V24" t="s">
+        <v>8</v>
+      </c>
+      <c r="W24" t="s">
+        <v>8</v>
+      </c>
+      <c r="X24" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y24" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z24" t="s">
+        <v>8</v>
+      </c>
+      <c r="AA24" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB24" t="s">
+        <v>8</v>
+      </c>
+      <c r="AC24" t="s">
+        <v>8</v>
+      </c>
+      <c r="AD24" t="s">
+        <v>8</v>
+      </c>
+      <c r="AE24" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:31">
+      <c r="A25" t="s">
         <v>3</v>
       </c>
-      <c r="B24" t="s">
-        <v>9</v>
-      </c>
-      <c r="C24" t="s">
-        <v>9</v>
-      </c>
-      <c r="D24" t="s">
-        <v>9</v>
-      </c>
-      <c r="E24" t="s">
-        <v>9</v>
-      </c>
-      <c r="F24" t="s">
-        <v>9</v>
-      </c>
-      <c r="G24" t="s">
-        <v>9</v>
-      </c>
-      <c r="H24" t="s">
-        <v>9</v>
-      </c>
-      <c r="I24" t="s">
-        <v>9</v>
-      </c>
-      <c r="J24" t="s">
-        <v>9</v>
-      </c>
-      <c r="K24" t="s">
-        <v>9</v>
-      </c>
-      <c r="L24" t="s">
-        <v>9</v>
-      </c>
-      <c r="M24" t="s">
-        <v>9</v>
-      </c>
-      <c r="N24" t="s">
-        <v>9</v>
-      </c>
-      <c r="O24" t="s">
-        <v>9</v>
-      </c>
-      <c r="P24" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q24" t="s">
-        <v>9</v>
-      </c>
-      <c r="R24" t="s">
-        <v>9</v>
-      </c>
-      <c r="S24" t="s">
-        <v>9</v>
-      </c>
-      <c r="T24" t="s">
-        <v>9</v>
-      </c>
-      <c r="U24" t="s">
-        <v>9</v>
-      </c>
-      <c r="V24" t="s">
-        <v>9</v>
-      </c>
-      <c r="W24" t="s">
-        <v>9</v>
-      </c>
-      <c r="X24" t="s">
-        <v>9</v>
-      </c>
-      <c r="Y24" t="s">
-        <v>9</v>
-      </c>
-      <c r="Z24" t="s">
-        <v>9</v>
-      </c>
-      <c r="AA24" t="s">
-        <v>9</v>
-      </c>
-      <c r="AB24" t="s">
-        <v>9</v>
-      </c>
-      <c r="AC24" t="s">
-        <v>9</v>
-      </c>
-      <c r="AD24" t="s">
-        <v>9</v>
-      </c>
-      <c r="AE24" t="s">
-        <v>9</v>
+      <c r="B25" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25" t="s">
+        <v>8</v>
+      </c>
+      <c r="D25" t="s">
+        <v>8</v>
+      </c>
+      <c r="E25" t="s">
+        <v>8</v>
+      </c>
+      <c r="F25" t="s">
+        <v>8</v>
+      </c>
+      <c r="G25" t="s">
+        <v>8</v>
+      </c>
+      <c r="H25" t="s">
+        <v>8</v>
+      </c>
+      <c r="I25" t="s">
+        <v>8</v>
+      </c>
+      <c r="J25" t="s">
+        <v>8</v>
+      </c>
+      <c r="K25" t="s">
+        <v>8</v>
+      </c>
+      <c r="L25" t="s">
+        <v>8</v>
+      </c>
+      <c r="M25" t="s">
+        <v>8</v>
+      </c>
+      <c r="N25" t="s">
+        <v>8</v>
+      </c>
+      <c r="O25" t="s">
+        <v>8</v>
+      </c>
+      <c r="P25" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>8</v>
+      </c>
+      <c r="R25" t="s">
+        <v>8</v>
+      </c>
+      <c r="S25" t="s">
+        <v>8</v>
+      </c>
+      <c r="T25" t="s">
+        <v>8</v>
+      </c>
+      <c r="U25" t="s">
+        <v>8</v>
+      </c>
+      <c r="V25" t="s">
+        <v>8</v>
+      </c>
+      <c r="W25" t="s">
+        <v>8</v>
+      </c>
+      <c r="X25" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y25" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AA25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AC25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AD25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AE25" t="s">
+        <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>4</v>
-      </c>
-      <c r="B25" t="s">
-        <v>9</v>
-      </c>
-      <c r="C25" t="s">
-        <v>9</v>
-      </c>
-      <c r="D25" t="s">
-        <v>9</v>
-      </c>
-      <c r="E25" t="s">
-        <v>9</v>
-      </c>
-      <c r="F25" t="s">
-        <v>9</v>
-      </c>
-      <c r="G25" t="s">
-        <v>9</v>
-      </c>
-      <c r="H25" t="s">
-        <v>9</v>
-      </c>
-      <c r="I25" t="s">
-        <v>9</v>
-      </c>
-      <c r="J25" t="s">
-        <v>9</v>
-      </c>
-      <c r="K25" t="s">
-        <v>9</v>
-      </c>
-      <c r="L25" t="s">
-        <v>9</v>
-      </c>
-      <c r="M25" t="s">
-        <v>9</v>
-      </c>
-      <c r="N25" t="s">
-        <v>9</v>
-      </c>
-      <c r="O25" t="s">
-        <v>9</v>
-      </c>
-      <c r="P25" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q25" t="s">
-        <v>9</v>
-      </c>
-      <c r="R25" t="s">
-        <v>9</v>
-      </c>
-      <c r="S25" t="s">
-        <v>9</v>
-      </c>
-      <c r="T25" t="s">
-        <v>9</v>
-      </c>
-      <c r="U25" t="s">
-        <v>9</v>
-      </c>
-      <c r="V25" t="s">
-        <v>9</v>
-      </c>
-      <c r="W25" t="s">
-        <v>9</v>
-      </c>
-      <c r="X25" t="s">
-        <v>9</v>
-      </c>
-      <c r="Y25" t="s">
-        <v>9</v>
-      </c>
-      <c r="Z25" t="s">
-        <v>9</v>
-      </c>
-      <c r="AA25" t="s">
-        <v>9</v>
-      </c>
-      <c r="AB25" t="s">
-        <v>9</v>
-      </c>
-      <c r="AC25" t="s">
-        <v>9</v>
-      </c>
-      <c r="AD25" t="s">
-        <v>9</v>
-      </c>
-      <c r="AE25" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="26" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:31">
       <c r="A26" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B26">
         <v>110.9</v>
@@ -3412,9 +3421,9 @@
         <v>135.4</v>
       </c>
     </row>
-    <row r="27" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:31">
       <c r="A27" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B27">
         <v>109.9</v>
@@ -3507,9 +3516,9 @@
         <v>134.19999999999999</v>
       </c>
     </row>
-    <row r="28" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:31">
       <c r="A28" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B28">
         <v>0</v>
@@ -3602,9 +3611,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:31">
       <c r="A29" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B29">
         <v>1</v>
@@ -3697,9 +3706,9 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="30" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:31">
       <c r="A30" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B30">
         <v>78.3</v>
@@ -3792,9 +3801,9 @@
         <v>45.7</v>
       </c>
     </row>
-    <row r="31" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:31">
       <c r="A31" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B31">
         <v>77.5</v>
@@ -3887,104 +3896,104 @@
         <v>45.2</v>
       </c>
     </row>
-    <row r="32" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:31">
       <c r="A32" t="s">
+        <v>2</v>
+      </c>
+      <c r="B32">
+        <v>0.1</v>
+      </c>
+      <c r="C32">
+        <v>0.1</v>
+      </c>
+      <c r="D32">
+        <v>0.1</v>
+      </c>
+      <c r="E32">
+        <v>0.1</v>
+      </c>
+      <c r="F32">
+        <v>0.1</v>
+      </c>
+      <c r="G32">
+        <v>0.1</v>
+      </c>
+      <c r="H32">
+        <v>0.1</v>
+      </c>
+      <c r="I32">
+        <v>0.1</v>
+      </c>
+      <c r="J32">
+        <v>0.1</v>
+      </c>
+      <c r="K32">
+        <v>0.1</v>
+      </c>
+      <c r="L32">
+        <v>0.1</v>
+      </c>
+      <c r="M32">
+        <v>0.1</v>
+      </c>
+      <c r="N32" t="s">
+        <v>8</v>
+      </c>
+      <c r="O32" t="s">
+        <v>8</v>
+      </c>
+      <c r="P32" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q32">
+        <v>0.1</v>
+      </c>
+      <c r="R32" t="s">
+        <v>8</v>
+      </c>
+      <c r="S32" t="s">
+        <v>8</v>
+      </c>
+      <c r="T32" t="s">
+        <v>8</v>
+      </c>
+      <c r="U32" t="s">
+        <v>8</v>
+      </c>
+      <c r="V32" t="s">
+        <v>8</v>
+      </c>
+      <c r="W32" t="s">
+        <v>8</v>
+      </c>
+      <c r="X32" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y32" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z32" t="s">
+        <v>8</v>
+      </c>
+      <c r="AA32" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB32" t="s">
+        <v>8</v>
+      </c>
+      <c r="AC32" t="s">
+        <v>8</v>
+      </c>
+      <c r="AD32" t="s">
+        <v>8</v>
+      </c>
+      <c r="AE32" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:31">
+      <c r="A33" t="s">
         <v>3</v>
-      </c>
-      <c r="B32">
-        <v>0.1</v>
-      </c>
-      <c r="C32">
-        <v>0.1</v>
-      </c>
-      <c r="D32">
-        <v>0.1</v>
-      </c>
-      <c r="E32">
-        <v>0.1</v>
-      </c>
-      <c r="F32">
-        <v>0.1</v>
-      </c>
-      <c r="G32">
-        <v>0.1</v>
-      </c>
-      <c r="H32">
-        <v>0.1</v>
-      </c>
-      <c r="I32">
-        <v>0.1</v>
-      </c>
-      <c r="J32">
-        <v>0.1</v>
-      </c>
-      <c r="K32">
-        <v>0.1</v>
-      </c>
-      <c r="L32">
-        <v>0.1</v>
-      </c>
-      <c r="M32">
-        <v>0.1</v>
-      </c>
-      <c r="N32" t="s">
-        <v>9</v>
-      </c>
-      <c r="O32" t="s">
-        <v>9</v>
-      </c>
-      <c r="P32" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q32">
-        <v>0.1</v>
-      </c>
-      <c r="R32" t="s">
-        <v>9</v>
-      </c>
-      <c r="S32" t="s">
-        <v>9</v>
-      </c>
-      <c r="T32" t="s">
-        <v>9</v>
-      </c>
-      <c r="U32" t="s">
-        <v>9</v>
-      </c>
-      <c r="V32" t="s">
-        <v>9</v>
-      </c>
-      <c r="W32" t="s">
-        <v>9</v>
-      </c>
-      <c r="X32" t="s">
-        <v>9</v>
-      </c>
-      <c r="Y32" t="s">
-        <v>9</v>
-      </c>
-      <c r="Z32" t="s">
-        <v>9</v>
-      </c>
-      <c r="AA32" t="s">
-        <v>9</v>
-      </c>
-      <c r="AB32" t="s">
-        <v>9</v>
-      </c>
-      <c r="AC32" t="s">
-        <v>9</v>
-      </c>
-      <c r="AD32" t="s">
-        <v>9</v>
-      </c>
-      <c r="AE32" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="33" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>4</v>
       </c>
       <c r="B33">
         <v>0.7</v>
@@ -4077,9 +4086,9 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="34" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:31">
       <c r="A34" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B34">
         <v>47</v>
@@ -4172,9 +4181,9 @@
         <v>40.4</v>
       </c>
     </row>
-    <row r="35" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:31">
       <c r="A35" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B35">
         <v>46.3</v>
@@ -4267,9 +4276,9 @@
         <v>35.9</v>
       </c>
     </row>
-    <row r="36" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:31">
       <c r="A36" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B36">
         <v>0.4</v>
@@ -4362,9 +4371,9 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="37" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:31">
       <c r="A37" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B37">
         <v>0.3</v>
@@ -4457,27 +4466,27 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="38" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:31">
       <c r="A38" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B38">
         <v>0</v>
       </c>
-      <c r="C38">
-        <v>0</v>
-      </c>
-      <c r="D38">
-        <v>0</v>
+      <c r="C38" t="s">
+        <v>8</v>
+      </c>
+      <c r="D38" t="s">
+        <v>8</v>
       </c>
       <c r="E38" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F38" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G38" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H38">
         <v>0.1</v>
@@ -4552,9 +4561,9 @@
         <v>3.9</v>
       </c>
     </row>
-    <row r="39" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:31">
       <c r="A39" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B39">
         <v>39</v>
@@ -4647,9 +4656,9 @@
         <v>40.799999999999997</v>
       </c>
     </row>
-    <row r="40" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:31">
       <c r="A40" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B40">
         <v>38.5</v>
@@ -4742,104 +4751,104 @@
         <v>40.200000000000003</v>
       </c>
     </row>
-    <row r="41" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:31">
       <c r="A41" t="s">
+        <v>2</v>
+      </c>
+      <c r="B41">
+        <v>0.1</v>
+      </c>
+      <c r="C41">
+        <v>0.1</v>
+      </c>
+      <c r="D41">
+        <v>0.1</v>
+      </c>
+      <c r="E41">
+        <v>0.1</v>
+      </c>
+      <c r="F41">
+        <v>0.1</v>
+      </c>
+      <c r="G41">
+        <v>0.1</v>
+      </c>
+      <c r="H41">
+        <v>0.1</v>
+      </c>
+      <c r="I41">
+        <v>0.1</v>
+      </c>
+      <c r="J41">
+        <v>0.1</v>
+      </c>
+      <c r="K41">
+        <v>0.1</v>
+      </c>
+      <c r="L41">
+        <v>0.1</v>
+      </c>
+      <c r="M41">
+        <v>0.1</v>
+      </c>
+      <c r="N41">
+        <v>0.1</v>
+      </c>
+      <c r="O41">
+        <v>0.1</v>
+      </c>
+      <c r="P41">
+        <v>0.1</v>
+      </c>
+      <c r="Q41">
+        <v>0.1</v>
+      </c>
+      <c r="R41">
+        <v>0.1</v>
+      </c>
+      <c r="S41">
+        <v>0.1</v>
+      </c>
+      <c r="T41">
+        <v>0.1</v>
+      </c>
+      <c r="U41">
+        <v>0.1</v>
+      </c>
+      <c r="V41">
+        <v>0.1</v>
+      </c>
+      <c r="W41">
+        <v>0.1</v>
+      </c>
+      <c r="X41">
+        <v>0.1</v>
+      </c>
+      <c r="Y41">
+        <v>0.1</v>
+      </c>
+      <c r="Z41">
+        <v>0.1</v>
+      </c>
+      <c r="AA41">
+        <v>0.1</v>
+      </c>
+      <c r="AB41">
+        <v>0.1</v>
+      </c>
+      <c r="AC41">
+        <v>0.1</v>
+      </c>
+      <c r="AD41">
+        <v>0.1</v>
+      </c>
+      <c r="AE41">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:31">
+      <c r="A42" t="s">
         <v>3</v>
-      </c>
-      <c r="B41">
-        <v>0.1</v>
-      </c>
-      <c r="C41">
-        <v>0.1</v>
-      </c>
-      <c r="D41">
-        <v>0.1</v>
-      </c>
-      <c r="E41">
-        <v>0.1</v>
-      </c>
-      <c r="F41">
-        <v>0.1</v>
-      </c>
-      <c r="G41">
-        <v>0.1</v>
-      </c>
-      <c r="H41">
-        <v>0.1</v>
-      </c>
-      <c r="I41">
-        <v>0.1</v>
-      </c>
-      <c r="J41">
-        <v>0.1</v>
-      </c>
-      <c r="K41">
-        <v>0.1</v>
-      </c>
-      <c r="L41">
-        <v>0.1</v>
-      </c>
-      <c r="M41">
-        <v>0.1</v>
-      </c>
-      <c r="N41">
-        <v>0.1</v>
-      </c>
-      <c r="O41">
-        <v>0.1</v>
-      </c>
-      <c r="P41">
-        <v>0.1</v>
-      </c>
-      <c r="Q41">
-        <v>0.1</v>
-      </c>
-      <c r="R41">
-        <v>0.1</v>
-      </c>
-      <c r="S41">
-        <v>0.1</v>
-      </c>
-      <c r="T41">
-        <v>0.1</v>
-      </c>
-      <c r="U41">
-        <v>0.1</v>
-      </c>
-      <c r="V41">
-        <v>0.1</v>
-      </c>
-      <c r="W41">
-        <v>0.1</v>
-      </c>
-      <c r="X41">
-        <v>0.1</v>
-      </c>
-      <c r="Y41">
-        <v>0.1</v>
-      </c>
-      <c r="Z41">
-        <v>0.1</v>
-      </c>
-      <c r="AA41">
-        <v>0.1</v>
-      </c>
-      <c r="AB41">
-        <v>0.1</v>
-      </c>
-      <c r="AC41">
-        <v>0.1</v>
-      </c>
-      <c r="AD41">
-        <v>0.1</v>
-      </c>
-      <c r="AE41">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>4</v>
       </c>
       <c r="B42">
         <v>0.3</v>
@@ -4932,9 +4941,9 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="43" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:31">
       <c r="A43" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B43">
         <v>0</v>
@@ -4955,7 +4964,7 @@
         <v>0</v>
       </c>
       <c r="H43" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I43">
         <v>0.1</v>
@@ -5027,104 +5036,104 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="44" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:31">
       <c r="A44" t="s">
+        <v>14</v>
+      </c>
+      <c r="B44">
+        <v>0.1</v>
+      </c>
+      <c r="C44">
+        <v>0.1</v>
+      </c>
+      <c r="D44">
+        <v>0.1</v>
+      </c>
+      <c r="E44">
+        <v>0.1</v>
+      </c>
+      <c r="F44">
+        <v>0.1</v>
+      </c>
+      <c r="G44">
+        <v>0.1</v>
+      </c>
+      <c r="H44">
+        <v>0.1</v>
+      </c>
+      <c r="I44" t="s">
+        <v>8</v>
+      </c>
+      <c r="J44" t="s">
+        <v>8</v>
+      </c>
+      <c r="K44" t="s">
+        <v>8</v>
+      </c>
+      <c r="L44" t="s">
+        <v>8</v>
+      </c>
+      <c r="M44" t="s">
+        <v>8</v>
+      </c>
+      <c r="N44" t="s">
+        <v>8</v>
+      </c>
+      <c r="O44" t="s">
+        <v>8</v>
+      </c>
+      <c r="P44" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q44" t="s">
+        <v>8</v>
+      </c>
+      <c r="R44" t="s">
+        <v>8</v>
+      </c>
+      <c r="S44">
+        <v>0.1</v>
+      </c>
+      <c r="T44" t="s">
+        <v>8</v>
+      </c>
+      <c r="U44" t="s">
+        <v>8</v>
+      </c>
+      <c r="V44" t="s">
+        <v>8</v>
+      </c>
+      <c r="W44" t="s">
+        <v>8</v>
+      </c>
+      <c r="X44" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y44" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z44">
+        <v>0.1</v>
+      </c>
+      <c r="AA44" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB44" t="s">
+        <v>8</v>
+      </c>
+      <c r="AC44">
+        <v>0.1</v>
+      </c>
+      <c r="AD44">
+        <v>0.1</v>
+      </c>
+      <c r="AE44">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:31">
+      <c r="A45" t="s">
         <v>15</v>
-      </c>
-      <c r="B44">
-        <v>0.1</v>
-      </c>
-      <c r="C44">
-        <v>0.1</v>
-      </c>
-      <c r="D44">
-        <v>0.1</v>
-      </c>
-      <c r="E44">
-        <v>0.1</v>
-      </c>
-      <c r="F44">
-        <v>0.1</v>
-      </c>
-      <c r="G44">
-        <v>0.1</v>
-      </c>
-      <c r="H44">
-        <v>0.1</v>
-      </c>
-      <c r="I44" t="s">
-        <v>9</v>
-      </c>
-      <c r="J44" t="s">
-        <v>9</v>
-      </c>
-      <c r="K44" t="s">
-        <v>9</v>
-      </c>
-      <c r="L44" t="s">
-        <v>9</v>
-      </c>
-      <c r="M44" t="s">
-        <v>9</v>
-      </c>
-      <c r="N44" t="s">
-        <v>9</v>
-      </c>
-      <c r="O44" t="s">
-        <v>9</v>
-      </c>
-      <c r="P44" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q44" t="s">
-        <v>9</v>
-      </c>
-      <c r="R44" t="s">
-        <v>9</v>
-      </c>
-      <c r="S44">
-        <v>0.1</v>
-      </c>
-      <c r="T44" t="s">
-        <v>9</v>
-      </c>
-      <c r="U44" t="s">
-        <v>9</v>
-      </c>
-      <c r="V44" t="s">
-        <v>9</v>
-      </c>
-      <c r="W44" t="s">
-        <v>9</v>
-      </c>
-      <c r="X44" t="s">
-        <v>9</v>
-      </c>
-      <c r="Y44" t="s">
-        <v>9</v>
-      </c>
-      <c r="Z44">
-        <v>0.1</v>
-      </c>
-      <c r="AA44" t="s">
-        <v>9</v>
-      </c>
-      <c r="AB44" t="s">
-        <v>9</v>
-      </c>
-      <c r="AC44">
-        <v>0.1</v>
-      </c>
-      <c r="AD44">
-        <v>0.1</v>
-      </c>
-      <c r="AE44">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
-        <v>16</v>
       </c>
       <c r="B45">
         <v>36</v>
@@ -5217,9 +5226,9 @@
         <v>53.7</v>
       </c>
     </row>
-    <row r="46" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:31">
       <c r="A46" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B46">
         <v>36</v>
@@ -5312,9 +5321,9 @@
         <v>53.7</v>
       </c>
     </row>
-    <row r="47" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:31">
       <c r="A47" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B47" s="1">
         <v>1517.9</v>
@@ -5407,9 +5416,9 @@
         <v>1871.7</v>
       </c>
     </row>
-    <row r="48" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:31">
       <c r="A48" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B48">
         <v>54.8</v>
@@ -5502,9 +5511,9 @@
         <v>26.4</v>
       </c>
     </row>
-    <row r="49" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:31">
       <c r="A49" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B49">
         <v>4.0999999999999996</v>
@@ -5597,9 +5606,9 @@
         <v>78.7</v>
       </c>
     </row>
-    <row r="50" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:31">
       <c r="A50" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B50">
         <v>0</v>

</xml_diff>